<commit_message>
Update Build List FIle
</commit_message>
<xml_diff>
--- a/Virpil ACE VPForce Build List.xlsx
+++ b/Virpil ACE VPForce Build List.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="90">
   <si>
     <t>Printed Parts List</t>
   </si>
@@ -124,28 +124,55 @@
     <t>15T, 12.7mm, HTD5</t>
   </si>
   <si>
+    <t>https://www.amazon.com/gp/product/B00J9TUH74</t>
+  </si>
+  <si>
+    <t>Drive Belt</t>
+  </si>
+  <si>
+    <t>570mm 114T, HTD5</t>
+  </si>
+  <si>
     <t>https://www.amazon.com/gp/product/B09TCZ59TX</t>
   </si>
   <si>
-    <t>Drive Belt</t>
-  </si>
-  <si>
-    <t>570mm 114T, HTD5</t>
+    <t>Power Supply</t>
+  </si>
+  <si>
+    <t>24v 10A</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/gp/product/B0993V49LH</t>
+  </si>
+  <si>
+    <t>Power Connector</t>
+  </si>
+  <si>
+    <t>5.5x2.5mm Female</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/gp/product/B07Y8KKSR1</t>
   </si>
   <si>
     <t>2040 T-Slot Extrusion</t>
   </si>
   <si>
-    <t>400mm</t>
-  </si>
-  <si>
-    <t>110mm</t>
+    <t>400mm pieces</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/gp/product/B099NBK1TD</t>
+  </si>
+  <si>
+    <t>110mm pieces</t>
   </si>
   <si>
     <t>2080 T-Slot Extrusion</t>
   </si>
   <si>
-    <t>105mm</t>
+    <t>105mm pieces</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/gp/product/B0B7HQRQ5G</t>
   </si>
   <si>
     <t>90 Degree Bracket - 2040</t>
@@ -260,7 +287,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -306,6 +333,10 @@
       <u/>
       <color rgb="FF0000FF"/>
     </font>
+    <font>
+      <u/>
+      <color rgb="FF0000FF"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -321,7 +352,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="30">
+  <borders count="31">
     <border/>
     <border>
       <left style="thick">
@@ -646,6 +677,17 @@
         <color rgb="FF000000"/>
       </left>
       <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thick">
         <color rgb="FF000000"/>
       </right>
       <top style="thin">
@@ -670,7 +712,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="62">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -803,27 +845,31 @@
     <xf borderId="28" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="14" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="29" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="center"/>
+    </xf>
     <xf borderId="26" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="9" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="27" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="14" fillId="2" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="14" fillId="2" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="27" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="13" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="13" fillId="2" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="14" fillId="2" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="14" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="14" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="14" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="29" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="14" fillId="2" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="14" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="30" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="12" fillId="2" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
@@ -1267,262 +1313,299 @@
         <v>6</v>
       </c>
       <c r="D22" s="46" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="47" t="s">
-        <v>40</v>
+      <c r="A23" s="42" t="s">
+        <v>41</v>
       </c>
       <c r="B23" s="18" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C23" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" s="43" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="44" t="s">
+        <v>44</v>
+      </c>
+      <c r="B24" s="45" t="s">
+        <v>45</v>
+      </c>
+      <c r="C24" s="45" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" s="46" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="47" t="s">
+        <v>47</v>
+      </c>
+      <c r="B25" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="C25" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="D23" s="48"/>
-    </row>
-    <row r="24">
-      <c r="A24" s="49"/>
-      <c r="B24" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="C24" s="18" t="s">
+      <c r="D25" s="48" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="49"/>
+      <c r="B26" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="C26" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="D24" s="48"/>
-    </row>
-    <row r="25">
-      <c r="A25" s="50" t="s">
-        <v>43</v>
-      </c>
-      <c r="B25" s="45" t="s">
-        <v>44</v>
-      </c>
-      <c r="C25" s="45" t="s">
+      <c r="D26" s="50"/>
+    </row>
+    <row r="27">
+      <c r="A27" s="51" t="s">
+        <v>51</v>
+      </c>
+      <c r="B27" s="45" t="s">
+        <v>52</v>
+      </c>
+      <c r="C27" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="D25" s="51"/>
-    </row>
-    <row r="26">
-      <c r="A26" s="52" t="s">
-        <v>45</v>
-      </c>
-      <c r="B26" s="53"/>
-      <c r="C26" s="18" t="s">
+      <c r="D27" s="52" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="53" t="s">
+        <v>54</v>
+      </c>
+      <c r="B28" s="54"/>
+      <c r="C28" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="D26" s="43" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="50" t="s">
-        <v>47</v>
-      </c>
-      <c r="B27" s="54"/>
-      <c r="C27" s="45" t="s">
+      <c r="D28" s="43" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="51" t="s">
+        <v>56</v>
+      </c>
+      <c r="B29" s="55"/>
+      <c r="C29" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="D27" s="55" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="52" t="s">
-        <v>49</v>
-      </c>
-      <c r="B28" s="53"/>
-      <c r="C28" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="D28" s="56" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" s="50" t="s">
-        <v>51</v>
-      </c>
-      <c r="B29" s="45" t="s">
-        <v>52</v>
-      </c>
-      <c r="C29" s="45" t="s">
-        <v>6</v>
-      </c>
-      <c r="D29" s="46" t="s">
-        <v>53</v>
+      <c r="D29" s="52" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="52" t="s">
-        <v>54</v>
-      </c>
-      <c r="B30" s="53"/>
+      <c r="A30" s="53" t="s">
+        <v>58</v>
+      </c>
+      <c r="B30" s="54"/>
       <c r="C30" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="D30" s="43" t="s">
-        <v>55</v>
+      <c r="D30" s="56" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="50" t="s">
-        <v>56</v>
+      <c r="A31" s="51" t="s">
+        <v>60</v>
       </c>
       <c r="B31" s="45" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="C31" s="45" t="s">
-        <v>58</v>
-      </c>
-      <c r="D31" s="55" t="s">
-        <v>59</v>
+        <v>6</v>
+      </c>
+      <c r="D31" s="46" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="52" t="s">
-        <v>60</v>
-      </c>
-      <c r="B32" s="18" t="s">
-        <v>61</v>
-      </c>
+      <c r="A32" s="53" t="s">
+        <v>63</v>
+      </c>
+      <c r="B32" s="54"/>
       <c r="C32" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="D32" s="19"/>
+        <v>6</v>
+      </c>
+      <c r="D32" s="43" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="33">
-      <c r="A33" s="50" t="s">
-        <v>63</v>
+      <c r="A33" s="51" t="s">
+        <v>65</v>
       </c>
       <c r="B33" s="45" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="C33" s="45" t="s">
-        <v>62</v>
-      </c>
-      <c r="D33" s="57"/>
+        <v>67</v>
+      </c>
+      <c r="D33" s="52" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="34">
-      <c r="A34" s="52" t="s">
-        <v>64</v>
+      <c r="A34" s="53" t="s">
+        <v>69</v>
       </c>
       <c r="B34" s="18" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="C34" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="D34" s="43" t="s">
-        <v>67</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="D34" s="19"/>
     </row>
     <row r="35">
-      <c r="A35" s="50" t="s">
-        <v>68</v>
+      <c r="A35" s="51" t="s">
+        <v>72</v>
       </c>
       <c r="B35" s="45" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C35" s="45" t="s">
-        <v>24</v>
-      </c>
-      <c r="D35" s="51"/>
+        <v>71</v>
+      </c>
+      <c r="D35" s="57"/>
     </row>
     <row r="36">
-      <c r="A36" s="52" t="s">
-        <v>70</v>
+      <c r="A36" s="53" t="s">
+        <v>73</v>
       </c>
       <c r="B36" s="18" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C36" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="D36" s="48"/>
+        <v>75</v>
+      </c>
+      <c r="D36" s="43" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="37">
-      <c r="A37" s="50" t="s">
-        <v>72</v>
+      <c r="A37" s="51" t="s">
+        <v>77</v>
       </c>
       <c r="B37" s="45" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="C37" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="D37" s="51"/>
+      <c r="D37" s="58"/>
     </row>
     <row r="38">
-      <c r="A38" s="52" t="s">
-        <v>74</v>
+      <c r="A38" s="53" t="s">
+        <v>79</v>
       </c>
       <c r="B38" s="18" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="C38" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="D38" s="48"/>
+      <c r="D38" s="59"/>
     </row>
     <row r="39">
-      <c r="A39" s="50" t="s">
-        <v>75</v>
+      <c r="A39" s="51" t="s">
+        <v>81</v>
       </c>
       <c r="B39" s="45" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="C39" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="D39" s="51"/>
+      <c r="D39" s="58"/>
     </row>
     <row r="40">
-      <c r="A40" s="52" t="s">
-        <v>77</v>
+      <c r="A40" s="53" t="s">
+        <v>83</v>
       </c>
       <c r="B40" s="18" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="C40" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="D40" s="48"/>
+      <c r="D40" s="59"/>
     </row>
     <row r="41">
-      <c r="A41" s="58" t="s">
-        <v>79</v>
-      </c>
-      <c r="B41" s="26" t="s">
-        <v>80</v>
-      </c>
-      <c r="C41" s="26" t="s">
+      <c r="A41" s="51" t="s">
+        <v>84</v>
+      </c>
+      <c r="B41" s="45" t="s">
+        <v>85</v>
+      </c>
+      <c r="C41" s="45" t="s">
+        <v>24</v>
+      </c>
+      <c r="D41" s="58"/>
+    </row>
+    <row r="42">
+      <c r="A42" s="53" t="s">
+        <v>86</v>
+      </c>
+      <c r="B42" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="C42" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="D42" s="59"/>
+    </row>
+    <row r="43">
+      <c r="A43" s="60" t="s">
+        <v>88</v>
+      </c>
+      <c r="B43" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C43" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="D41" s="59"/>
+      <c r="D43" s="61"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="A1:C1"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="A6:A10"/>
     <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A23:A24"/>
     <mergeCell ref="A18:D18"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="D25:D26"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="D20"/>
     <hyperlink r:id="rId2" ref="D21"/>
     <hyperlink r:id="rId3" ref="D22"/>
-    <hyperlink r:id="rId4" ref="D26"/>
-    <hyperlink r:id="rId5" ref="D27"/>
-    <hyperlink r:id="rId6" ref="D28"/>
-    <hyperlink r:id="rId7" ref="D29"/>
-    <hyperlink r:id="rId8" ref="D30"/>
-    <hyperlink r:id="rId9" ref="D31"/>
-    <hyperlink r:id="rId10" ref="D34"/>
+    <hyperlink r:id="rId4" ref="D23"/>
+    <hyperlink r:id="rId5" ref="D24"/>
+    <hyperlink r:id="rId6" ref="D25"/>
+    <hyperlink r:id="rId7" ref="D27"/>
+    <hyperlink r:id="rId8" ref="D28"/>
+    <hyperlink r:id="rId9" ref="D29"/>
+    <hyperlink r:id="rId10" ref="D30"/>
+    <hyperlink r:id="rId11" ref="D31"/>
+    <hyperlink r:id="rId12" ref="D32"/>
+    <hyperlink r:id="rId13" ref="D33"/>
+    <hyperlink r:id="rId14" ref="D36"/>
   </hyperlinks>
-  <drawing r:id="rId11"/>
+  <drawing r:id="rId15"/>
 </worksheet>
 </file>
</xml_diff>